<commit_message>
fixing the same typo in the template sheet...
</commit_message>
<xml_diff>
--- a/result_table_templates/PscOptoStats.xlsx
+++ b/result_table_templates/PscOptoStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D0A806-4752-45B1-A478-FF7D1F763B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2C930A-7FEB-4090-B04E-F82BB1C6BA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="19200" windowHeight="9840" xr2:uid="{4E5C92F6-82B9-4F97-8A34-069F2EAB3F7A}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4E5C92F6-82B9-4F97-8A34-069F2EAB3F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="pscStats" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>double</t>
   </si>
   <si>
-    <t>pcs_frequency</t>
-  </si>
-  <si>
     <t>number of psc/total time elapsed</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>1 if train, 0 if not</t>
+  </si>
+  <si>
+    <t>psc_frequency</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -545,7 +545,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -556,68 +556,68 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>